<commit_message>
updated rubric, apparently didn't get saved
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="82">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -925,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="H4" s="5">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91))</f>
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I4" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
@@ -1066,11 +1066,11 @@
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1089,10 +1089,12 @@
       <c r="E5" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G5" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>27</v>
@@ -1121,7 +1123,9 @@
       <c r="D6" s="5">
         <v>5</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="F6" s="3"/>
       <c r="G6" s="8">
         <f t="shared" si="0"/>
@@ -1129,7 +1133,7 @@
       </c>
       <c r="H6" s="5">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91)  &gt; 22, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) - 22,0)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I6" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) - 22,0)</f>
@@ -1199,11 +1203,11 @@
       </c>
       <c r="H8" s="10">
         <f>H4+IF(H4 &lt; 22, IF(K4+H4 &gt; 22, 22- H4, K4),0)</f>
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I8" s="9">
         <f>I4+IF(I4 &lt; 22, IF(H10+I4 &gt; 22, 22- I4, H10),0)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J8" s="9">
         <f>J4+IF(J4 &lt; 22, IF(I10+J4 &gt; 22, 22- J4, I10),0)</f>
@@ -1264,7 +1268,7 @@
       </c>
       <c r="H10" s="5">
         <f>IF(K4+H4 - 22 &gt; 0, K4+H4 - 22, 0)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
@@ -1422,10 +1426,12 @@
       <c r="E18" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F18" s="3"/>
+      <c r="F18" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G18" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -1686,10 +1692,12 @@
       <c r="E30" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F30" s="3"/>
+      <c r="F30" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G30" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -1711,7 +1719,7 @@
         <v>3</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="8">
@@ -1738,7 +1746,7 @@
         <v>3</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="8">
@@ -1765,7 +1773,7 @@
         <v>1</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="8">
@@ -2216,14 +2224,12 @@
         <v>3</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>78</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="F54" s="3"/>
       <c r="G54" s="8">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>

</xml_diff>

<commit_message>
New vertex and pixel shader with all of the lights combined, still needs some work.
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -35,7 +35,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F54" authorId="0">
+    <comment ref="F30" authorId="0">
       <text>
         <r>
           <rPr>
@@ -45,7 +45,42 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Press I to check
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+The flat plane has directional light
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F31" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+The pyramid has Point lights, one on each side
 </t>
         </r>
       </text>
@@ -107,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="85">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -405,6 +440,15 @@
   </si>
   <si>
     <t>http://www.directxtutorial.com/Lesson.aspx?lessonid=11-4-4</t>
+  </si>
+  <si>
+    <t>http://www.braynzarsoft.net/index.php?p=D3D11SIMPLELIGHT</t>
+  </si>
+  <si>
+    <t>http://www.rastertek.com/dx11tut30.html</t>
+  </si>
+  <si>
+    <t>III</t>
   </si>
 </sst>
 </file>
@@ -925,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1058,7 +1102,7 @@
       </c>
       <c r="I4" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="J4" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
@@ -1070,7 +1114,7 @@
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1195,7 +1239,9 @@
       <c r="D8" s="5">
         <v>5</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="F8" s="3"/>
       <c r="G8" s="8">
         <f t="shared" si="0"/>
@@ -1207,11 +1253,11 @@
       </c>
       <c r="I8" s="9">
         <f>I4+IF(I4 &lt; 22, IF(H10+I4 &gt; 22, 22- I4, H10),0)</f>
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="J8" s="9">
         <f>J4+IF(J4 &lt; 22, IF(I10+J4 &gt; 22, 22- J4, I10),0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1229,7 +1275,9 @@
       <c r="D9" s="5">
         <v>2</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="F9" s="3"/>
       <c r="G9" s="8">
         <f xml:space="preserve"> IF(EXACT(F9,"X"),IF(EXACT(E9,"I"),$B9,IF(EXACT(E9,"II"),$C9,IF(EXACT(E9,"III"),$D9,0))),0)</f>
@@ -1260,7 +1308,9 @@
       <c r="D10" s="5">
         <v>2</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="F10" s="3"/>
       <c r="G10" s="8">
         <f xml:space="preserve"> IF(EXACT(F10,"X"),IF(EXACT(E10,"I"),$B10,IF(EXACT(E10,"II"),$C10,IF(EXACT(E10,"III"),$D10,0))),0)</f>
@@ -1272,7 +1322,7 @@
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
@@ -1294,7 +1344,9 @@
       <c r="D11" s="5">
         <v>2</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="F11" s="3"/>
       <c r="G11" s="8">
         <f xml:space="preserve"> IF(EXACT(F11,"X"),IF(EXACT(E11,"I"),$B11,IF(EXACT(E11,"II"),$C11,IF(EXACT(E11,"III"),$D11,0))),0)</f>
@@ -1452,7 +1504,9 @@
       <c r="D19" s="5">
         <v>3</v>
       </c>
-      <c r="E19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="F19" s="3"/>
       <c r="G19" s="8">
         <f t="shared" si="0"/>
@@ -1477,7 +1531,9 @@
       <c r="D20" s="5">
         <v>5</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="F20" s="3"/>
       <c r="G20" s="8">
         <f t="shared" si="0"/>
@@ -1502,7 +1558,9 @@
       <c r="D21" s="5">
         <v>3</v>
       </c>
-      <c r="E21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="F21" s="3"/>
       <c r="G21" s="8">
         <f t="shared" si="0"/>
@@ -1552,11 +1610,15 @@
       <c r="D23" s="5">
         <v>4</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="3"/>
+      <c r="E23" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G23" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
@@ -1577,7 +1639,9 @@
       <c r="D24" s="5">
         <v>5</v>
       </c>
-      <c r="E24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="F24" s="3"/>
       <c r="G24" s="8">
         <f t="shared" si="0"/>
@@ -1721,10 +1785,12 @@
       <c r="E31" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F31" s="3"/>
+      <c r="F31" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G31" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -1775,10 +1841,12 @@
       <c r="E33" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F33" s="3"/>
+      <c r="F33" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G33" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
@@ -1799,7 +1867,9 @@
       <c r="D34" s="5">
         <v>1</v>
       </c>
-      <c r="E34" s="2"/>
+      <c r="E34" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="F34" s="3"/>
       <c r="G34" s="8">
         <f t="shared" si="0"/>
@@ -1824,7 +1894,9 @@
       <c r="D35" s="5">
         <v>1</v>
       </c>
-      <c r="E35" s="2"/>
+      <c r="E35" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="F35" s="3"/>
       <c r="G35" s="8">
         <f t="shared" si="0"/>
@@ -1849,7 +1921,9 @@
       <c r="D36" s="5">
         <v>2</v>
       </c>
-      <c r="E36" s="2"/>
+      <c r="E36" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="F36" s="3"/>
       <c r="G36" s="8">
         <f t="shared" ref="G36:G67" si="1" xml:space="preserve"> IF(EXACT(F36,"X"),IF(EXACT(E36,"I"),$B36,IF(EXACT(E36,"II"),$C36,IF(EXACT(E36,"III"),$D36,0))),0)</f>
@@ -1874,7 +1948,9 @@
       <c r="D37" s="5">
         <v>3</v>
       </c>
-      <c r="E37" s="2"/>
+      <c r="E37" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="F37" s="3"/>
       <c r="G37" s="8">
         <f t="shared" si="1"/>
@@ -1899,7 +1975,9 @@
       <c r="D38" s="5">
         <v>3</v>
       </c>
-      <c r="E38" s="2"/>
+      <c r="E38" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="F38" s="3"/>
       <c r="G38" s="8">
         <f t="shared" si="1"/>
@@ -1924,7 +2002,9 @@
       <c r="D39" s="5">
         <v>3</v>
       </c>
-      <c r="E39" s="2"/>
+      <c r="E39" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="F39" s="3"/>
       <c r="G39" s="8">
         <f t="shared" si="1"/>
@@ -1949,7 +2029,9 @@
       <c r="D40" s="5">
         <v>3</v>
       </c>
-      <c r="E40" s="2"/>
+      <c r="E40" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="F40" s="3"/>
       <c r="G40" s="8">
         <f t="shared" si="1"/>
@@ -2044,7 +2126,9 @@
       <c r="D45" s="5">
         <v>5</v>
       </c>
-      <c r="E45" s="2"/>
+      <c r="E45" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="F45" s="3"/>
       <c r="G45" s="8">
         <f t="shared" si="1"/>
@@ -2069,7 +2153,9 @@
       <c r="D46" s="5">
         <v>3</v>
       </c>
-      <c r="E46" s="2"/>
+      <c r="E46" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="F46" s="3"/>
       <c r="G46" s="8">
         <f t="shared" si="1"/>
@@ -2094,7 +2180,9 @@
       <c r="D47" s="5">
         <v>5</v>
       </c>
-      <c r="E47" s="2"/>
+      <c r="E47" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="F47" s="3"/>
       <c r="G47" s="8">
         <f t="shared" si="1"/>
@@ -2226,10 +2314,12 @@
       <c r="E54" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F54" s="3"/>
+      <c r="F54" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G54" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
@@ -2250,7 +2340,9 @@
       <c r="D55" s="5">
         <v>3</v>
       </c>
-      <c r="E55" s="2"/>
+      <c r="E55" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="F55" s="3"/>
       <c r="G55" s="8">
         <f t="shared" si="1"/>
@@ -2275,7 +2367,9 @@
       <c r="D56" s="5">
         <v>5</v>
       </c>
-      <c r="E56" s="2"/>
+      <c r="E56" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="F56" s="3"/>
       <c r="G56" s="8">
         <f t="shared" si="1"/>
@@ -2300,7 +2394,9 @@
       <c r="D57" s="5">
         <v>5</v>
       </c>
-      <c r="E57" s="2"/>
+      <c r="E57" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="F57" s="3"/>
       <c r="G57" s="8">
         <f t="shared" si="1"/>
@@ -2504,7 +2600,9 @@
       <c r="D67" s="5">
         <v>5</v>
       </c>
-      <c r="E67" s="2"/>
+      <c r="E67" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="F67" s="3"/>
       <c r="G67" s="8">
         <f t="shared" si="1"/>
@@ -2529,7 +2627,9 @@
       <c r="D68" s="5">
         <v>5</v>
       </c>
-      <c r="E68" s="2"/>
+      <c r="E68" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="F68" s="3"/>
       <c r="G68" s="8">
         <f t="shared" ref="G68:G85" si="2" xml:space="preserve"> IF(EXACT(F68,"X"),IF(EXACT(E68,"I"),$B68,IF(EXACT(E68,"II"),$C68,IF(EXACT(E68,"III"),$D68,0))),0)</f>
@@ -2658,7 +2758,9 @@
       <c r="D75" s="5">
         <v>5</v>
       </c>
-      <c r="E75" s="2"/>
+      <c r="E75" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="F75" s="3"/>
       <c r="G75" s="8">
         <f t="shared" si="2"/>
@@ -2916,7 +3018,9 @@
       <c r="C90" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D90" s="3"/>
+      <c r="D90" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="E90" s="3"/>
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
@@ -2936,7 +3040,9 @@
       <c r="C91" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D91" s="3"/>
+      <c r="D91" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="E91" s="3"/>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
@@ -2990,10 +3096,14 @@
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97" s="16"/>
+      <c r="A97" s="16" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98" s="16"/>
+      <c r="A98" s="16" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" s="16"/>

</xml_diff>

<commit_message>
Second viewport added, started messing with the viewport
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="85">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -969,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="I4" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J4" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
@@ -1114,7 +1114,7 @@
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1257,7 +1257,7 @@
       </c>
       <c r="J8" s="9">
         <f>J4+IF(J4 &lt; 22, IF(I10+J4 &gt; 22, 22- J4, I10),0)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1322,7 +1322,7 @@
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
@@ -2343,10 +2343,12 @@
       <c r="E55" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F55" s="3"/>
+      <c r="F55" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G55" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
@@ -3184,7 +3186,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
updated what I did
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="85">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -969,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1102,19 +1102,19 @@
       </c>
       <c r="I4" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J4" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="I6" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) - 22,0)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J6" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) - 22,0)</f>
@@ -1190,7 +1190,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="9">
         <f>IF(L4 &gt; 66, SUM(-66,L4),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -1257,7 +1257,7 @@
       </c>
       <c r="J8" s="9">
         <f>J4+IF(J4 &lt; 22, IF(I10+J4 &gt; 22, 22- J4, I10),0)</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1309,7 +1309,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="8">
@@ -1318,15 +1318,15 @@
       </c>
       <c r="H10" s="5">
         <f>IF(K4+H4 - 22 &gt; 0, K4+H4 - 22, 0)</f>
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1814,10 +1814,12 @@
       <c r="E32" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F32" s="3"/>
+      <c r="F32" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G32" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
@@ -1870,10 +1872,12 @@
       <c r="E34" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F34" s="3"/>
+      <c r="F34" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G34" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
@@ -1897,10 +1901,12 @@
       <c r="E35" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F35" s="3"/>
+      <c r="F35" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G35" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
@@ -1924,10 +1930,12 @@
       <c r="E36" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F36" s="3"/>
+      <c r="F36" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G36" s="8">
         <f t="shared" ref="G36:G67" si="1" xml:space="preserve"> IF(EXACT(F36,"X"),IF(EXACT(E36,"I"),$B36,IF(EXACT(E36,"II"),$C36,IF(EXACT(E36,"III"),$D36,0))),0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
@@ -2032,10 +2040,12 @@
       <c r="E40" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F40" s="3"/>
+      <c r="F40" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G40" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
@@ -2372,10 +2382,12 @@
       <c r="E56" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F56" s="3"/>
+      <c r="F56" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G56" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
@@ -2605,10 +2617,12 @@
       <c r="E67" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F67" s="3"/>
+      <c r="F67" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G67" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
@@ -3186,7 +3200,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Pushed the wrong folder... this is the real one
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="85">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -969,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1110,11 +1110,11 @@
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="I6" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) - 22,0)</f>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="J6" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) - 22,0)</f>
@@ -1190,7 +1190,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="9">
         <f>IF(L4 &gt; 66, SUM(-66,L4),0)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -1318,15 +1318,15 @@
       </c>
       <c r="H10" s="5">
         <f>IF(K4+H4 - 22 &gt; 0, K4+H4 - 22, 0)</f>
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -2380,7 +2380,7 @@
         <v>5</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>78</v>
@@ -2411,10 +2411,12 @@
       <c r="E57" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F57" s="3"/>
+      <c r="F57" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G57" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>

</xml_diff>

<commit_message>
added some cool things, fixed some old ones
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -32,6 +32,32 @@
             <charset val="1"/>
           </rPr>
           <t>Fill out name and repo address then submit to intial turn in on the graphics II sidekick.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F24" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+From the beginning point, you can look through 3 transparent objects, Once I get a sort in there, it should stay sorted.
+Also, not sure if the transparent tree leaves count.
+</t>
         </r>
       </text>
     </comment>
@@ -81,6 +107,81 @@
           </rPr>
           <t xml:space="preserve">
 The pyramid has Point lights, one on each side
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F32" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+I turned this off so you can see the other lights and the specular
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F40" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+the spot light rotates the camera and causes spec changes, but the spec is working correctly
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F54" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Multiple samples are taken and the state flags MS and AA as true.
 </t>
         </r>
       </text>
@@ -969,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1110,11 +1211,11 @@
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1168,7 +1269,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="8">
@@ -1177,11 +1278,11 @@
       </c>
       <c r="H6" s="5">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91)  &gt; 22, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) - 22,0)</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I6" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) - 22,0)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="J6" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) - 22,0)</f>
@@ -1190,7 +1291,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="9">
         <f>IF(L4 &gt; 66, SUM(-66,L4),0)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -1207,7 +1308,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="8">
@@ -1318,15 +1419,15 @@
       </c>
       <c r="H10" s="5">
         <f>IF(K4+H4 - 22 &gt; 0, K4+H4 - 22, 0)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1585,7 +1686,9 @@
       <c r="D22" s="5">
         <v>3</v>
       </c>
-      <c r="E22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="F22" s="3"/>
       <c r="G22" s="8">
         <f t="shared" si="0"/>
@@ -1642,10 +1745,12 @@
       <c r="E24" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F24" s="3"/>
+      <c r="F24" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G24" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
@@ -1754,14 +1859,14 @@
         <v>3</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>78</v>
       </c>
       <c r="G30" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -2353,12 +2458,10 @@
       <c r="E55" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F55" s="3" t="s">
-        <v>78</v>
-      </c>
+      <c r="F55" s="3"/>
       <c r="G55" s="8">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
@@ -2408,15 +2511,11 @@
       <c r="D57" s="5">
         <v>5</v>
       </c>
-      <c r="E57" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>78</v>
-      </c>
+      <c r="E57" s="2"/>
+      <c r="F57" s="3"/>
       <c r="G57" s="8">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
@@ -2646,12 +2745,14 @@
         <v>5</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F68" s="3"/>
+        <v>84</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G68" s="8">
         <f t="shared" ref="G68:G85" si="2" xml:space="preserve"> IF(EXACT(F68,"X"),IF(EXACT(E68,"I"),$B68,IF(EXACT(E68,"II"),$C68,IF(EXACT(E68,"III"),$D68,0))),0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>

</xml_diff>

<commit_message>
cleaned up code a bit, got 3 transparent textures ding their thing.
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -55,8 +55,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-From the beginning point, you can look through 3 transparent objects, Once I get a sort in there, it should stay sorted.
-Also, not sure if the transparent tree leaves count.
+From the beginning point, you can look through 3 transparent objects
+Also, transparent tree leaves.
 </t>
         </r>
       </text>
@@ -238,12 +238,38 @@
         </r>
       </text>
     </comment>
+    <comment ref="F68" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Can look through three transparent object
+with sorted depth blending
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="86">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -550,6 +576,9 @@
   </si>
   <si>
     <t>III</t>
+  </si>
+  <si>
+    <t>http://www.braynzarsoft.net/index.php?p=D3D11BLENDING</t>
   </si>
 </sst>
 </file>
@@ -1070,8 +1099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1207,7 +1236,7 @@
       </c>
       <c r="J4" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
@@ -1215,7 +1244,7 @@
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1268,9 +1297,7 @@
       <c r="D6" s="5">
         <v>5</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>84</v>
-      </c>
+      <c r="E6" s="2"/>
       <c r="F6" s="3"/>
       <c r="G6" s="8">
         <f t="shared" si="0"/>
@@ -1291,7 +1318,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="9">
         <f>IF(L4 &gt; 66, SUM(-66,L4),0)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -1307,9 +1334,7 @@
       <c r="D7" s="5">
         <v>4</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>84</v>
-      </c>
+      <c r="E7" s="2"/>
       <c r="F7" s="3"/>
       <c r="G7" s="8">
         <f t="shared" si="0"/>
@@ -1376,9 +1401,7 @@
       <c r="D9" s="5">
         <v>2</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>84</v>
-      </c>
+      <c r="E9" s="2"/>
       <c r="F9" s="3"/>
       <c r="G9" s="8">
         <f xml:space="preserve"> IF(EXACT(F9,"X"),IF(EXACT(E9,"I"),$B9,IF(EXACT(E9,"II"),$C9,IF(EXACT(E9,"III"),$D9,0))),0)</f>
@@ -1409,9 +1432,7 @@
       <c r="D10" s="5">
         <v>2</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>84</v>
-      </c>
+      <c r="E10" s="2"/>
       <c r="F10" s="3"/>
       <c r="G10" s="8">
         <f xml:space="preserve"> IF(EXACT(F10,"X"),IF(EXACT(E10,"I"),$B10,IF(EXACT(E10,"II"),$C10,IF(EXACT(E10,"III"),$D10,0))),0)</f>
@@ -1427,7 +1448,7 @@
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1445,9 +1466,7 @@
       <c r="D11" s="5">
         <v>2</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>84</v>
-      </c>
+      <c r="E11" s="2"/>
       <c r="F11" s="3"/>
       <c r="G11" s="8">
         <f xml:space="preserve"> IF(EXACT(F11,"X"),IF(EXACT(E11,"I"),$B11,IF(EXACT(E11,"II"),$C11,IF(EXACT(E11,"III"),$D11,0))),0)</f>
@@ -3140,7 +3159,9 @@
       <c r="D90" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E90" s="3"/>
+      <c r="E90" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
       <c r="H90" s="5"/>
@@ -3162,7 +3183,9 @@
       <c r="D91" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E91" s="3"/>
+      <c r="E91" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
       <c r="H91" s="5"/>
@@ -3225,7 +3248,9 @@
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99" s="16"/>
+      <c r="A99" s="16" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" s="16"/>

</xml_diff>

<commit_message>
got render to texture to work a lot better
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -269,7 +269,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="87">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -579,6 +579,9 @@
   </si>
   <si>
     <t>http://www.braynzarsoft.net/index.php?p=D3D11BLENDING</t>
+  </si>
+  <si>
+    <t>http://www.braynzarsoft.net/index.php?p=D3D11CLIPPING</t>
   </si>
 </sst>
 </file>
@@ -1099,8 +1102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1236,7 +1239,7 @@
       </c>
       <c r="J4" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
@@ -1244,7 +1247,7 @@
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1318,7 +1321,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="9">
         <f>IF(L4 &gt; 66, SUM(-66,L4),0)</f>
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -1448,7 +1451,7 @@
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1654,10 +1657,12 @@
       <c r="E20" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F20" s="3"/>
+      <c r="F20" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G20" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -2474,9 +2479,7 @@
       <c r="D55" s="5">
         <v>3</v>
       </c>
-      <c r="E55" s="2" t="s">
-        <v>79</v>
-      </c>
+      <c r="E55" s="2"/>
       <c r="F55" s="3"/>
       <c r="G55" s="8">
         <f t="shared" si="1"/>
@@ -3253,7 +3256,9 @@
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100" s="16"/>
+      <c r="A100" s="16" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" s="16"/>
@@ -3328,7 +3333,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
This is up to date, with render to texture added
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -269,7 +269,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="87">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -1102,8 +1102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1368,9 +1368,7 @@
       <c r="D8" s="5">
         <v>5</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>84</v>
-      </c>
+      <c r="E8" s="2"/>
       <c r="F8" s="3"/>
       <c r="G8" s="8">
         <f t="shared" si="0"/>
@@ -1683,9 +1681,7 @@
       <c r="D21" s="5">
         <v>3</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>84</v>
-      </c>
+      <c r="E21" s="2"/>
       <c r="F21" s="3"/>
       <c r="G21" s="8">
         <f t="shared" si="0"/>
@@ -3333,7 +3329,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
pushing before I break everything, attempting to add normal mapping.
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="13752" windowHeight="2700"/>
+    <workbookView xWindow="60" yWindow="-36" windowWidth="22980" windowHeight="5736"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1102,8 +1102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="H4" s="5">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91))</f>
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="I4" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
@@ -1243,11 +1243,11 @@
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1264,14 +1264,14 @@
         <v>3</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>78</v>
       </c>
       <c r="G5" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>27</v>
@@ -1308,11 +1308,11 @@
       </c>
       <c r="H6" s="5">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91)  &gt; 22, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) - 22,0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I6" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) - 22,0)</f>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J6" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) - 22,0)</f>
@@ -1321,7 +1321,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="9">
         <f>IF(L4 &gt; 66, SUM(-66,L4),0)</f>
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -1441,15 +1441,15 @@
       </c>
       <c r="H10" s="5">
         <f>IF(K4+H4 - 22 &gt; 0, K4+H4 - 22, 0)</f>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1597,14 +1597,14 @@
         <v>3</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>78</v>
       </c>
       <c r="G18" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -3329,7 +3329,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
mentioned the light switch in the rubric
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -155,7 +155,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-I turned this off so you can see the other lights and the specular
+use 'O' to switch on and off
 </t>
         </r>
       </text>
@@ -317,7 +317,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="88">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -1154,7 +1154,7 @@
   <dimension ref="A1:L117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2136,9 +2136,7 @@
       <c r="D37" s="5">
         <v>3</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>84</v>
-      </c>
+      <c r="E37" s="2"/>
       <c r="F37" s="3"/>
       <c r="G37" s="8">
         <f t="shared" si="1"/>
@@ -2163,9 +2161,7 @@
       <c r="D38" s="5">
         <v>3</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>84</v>
-      </c>
+      <c r="E38" s="2"/>
       <c r="F38" s="3"/>
       <c r="G38" s="8">
         <f t="shared" si="1"/>
@@ -3388,7 +3384,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>